<commit_message>
Created PDF and PNG file for data
Also added a README for week 2
</commit_message>
<xml_diff>
--- a/week1/library.xlsx
+++ b/week1/library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8299614b0b0b5a34/Documents/BYU-Idaho/TA/ITM 220-SQL/clarkprep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8299614b0b0b5a34/Documents/BYU-Idaho/TA/ITM 220-SQL/new_itm220/github/itm220student/week1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC104854119F4D9A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C67A329F-5B9F-4C52-9922-918681207BDD}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_F25DC773A252ABDACC104854119F4D9A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2126B001-27CB-40E8-9492-33554B515BAF}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,11 +538,16 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -944,5 +949,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>